<commit_message>
BugFix: - Fixed: memory error when search Thermo LC-MS > 30 min
</commit_message>
<xml_diff>
--- a/ConfigurationFiles/01-FA_Whitelist_TG-DG.xlsx
+++ b/ConfigurationFiles/01-FA_Whitelist_TG-DG.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{77F7DEFB-9296-4977-8EFA-7E678A4DE469}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20160" windowHeight="8472"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20160" windowHeight="8475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="69">
   <si>
     <t>FattyAcid</t>
   </si>
@@ -231,7 +232,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -542,19 +543,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F53" sqref="F53"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B58" sqref="B57:B58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -577,7 +578,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>63</v>
       </c>
@@ -597,7 +598,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>64</v>
       </c>
@@ -617,7 +618,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>65</v>
       </c>
@@ -637,7 +638,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>66</v>
       </c>
@@ -657,7 +658,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>41</v>
       </c>
@@ -677,7 +678,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>67</v>
       </c>
@@ -697,7 +698,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -717,7 +718,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>62</v>
       </c>
@@ -737,7 +738,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -757,7 +758,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>45</v>
       </c>
@@ -777,7 +778,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>42</v>
       </c>
@@ -797,7 +798,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>56</v>
       </c>
@@ -817,7 +818,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>57</v>
       </c>
@@ -837,7 +838,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -857,7 +858,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -877,7 +878,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>50</v>
       </c>
@@ -897,7 +898,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>43</v>
       </c>
@@ -917,7 +918,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>54</v>
       </c>
@@ -937,7 +938,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>55</v>
       </c>
@@ -957,7 +958,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>1</v>
       </c>
@@ -980,7 +981,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>29</v>
       </c>
@@ -1000,7 +1001,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>49</v>
       </c>
@@ -1020,7 +1021,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>44</v>
       </c>
@@ -1040,7 +1041,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>46</v>
       </c>
@@ -1060,7 +1061,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>53</v>
       </c>
@@ -1080,7 +1081,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>2</v>
       </c>
@@ -1103,7 +1104,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>3</v>
       </c>
@@ -1126,7 +1127,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>4</v>
       </c>
@@ -1149,7 +1150,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>5</v>
       </c>
@@ -1172,7 +1173,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -1192,7 +1193,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>47</v>
       </c>
@@ -1212,7 +1213,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>48</v>
       </c>
@@ -1232,7 +1233,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>52</v>
       </c>
@@ -1252,7 +1253,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>24</v>
       </c>
@@ -1272,7 +1273,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>31</v>
       </c>
@@ -1292,7 +1293,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>32</v>
       </c>
@@ -1312,7 +1313,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>6</v>
       </c>
@@ -1335,7 +1336,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>7</v>
       </c>
@@ -1358,7 +1359,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>8</v>
       </c>
@@ -1381,7 +1382,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>25</v>
       </c>
@@ -1401,7 +1402,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>33</v>
       </c>
@@ -1421,7 +1422,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>34</v>
       </c>
@@ -1441,7 +1442,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>35</v>
       </c>
@@ -1461,7 +1462,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>9</v>
       </c>
@@ -1484,7 +1485,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>10</v>
       </c>
@@ -1507,7 +1508,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>11</v>
       </c>
@@ -1527,7 +1528,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>51</v>
       </c>
@@ -1544,7 +1545,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>26</v>
       </c>
@@ -1561,7 +1562,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>36</v>
       </c>
@@ -1578,7 +1579,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>37</v>
       </c>
@@ -1595,7 +1596,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>38</v>
       </c>
@@ -1612,7 +1613,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>68</v>
       </c>
@@ -1629,7 +1630,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>27</v>
       </c>
@@ -1646,7 +1647,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>39</v>
       </c>
@@ -1663,7 +1664,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>40</v>
       </c>
@@ -1680,15 +1681,21 @@
         <v>18</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>12</v>
       </c>
+      <c r="B57" t="s">
+        <v>18</v>
+      </c>
       <c r="E57" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F57" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>13</v>
       </c>
@@ -1698,8 +1705,11 @@
       <c r="E58" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F58" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>14</v>
       </c>
@@ -1709,8 +1719,11 @@
       <c r="E59" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F59" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>15</v>
       </c>
@@ -1720,8 +1733,11 @@
       <c r="E60" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F60" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>16</v>
       </c>
@@ -1731,8 +1747,11 @@
       <c r="E61" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F61" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>17</v>
       </c>
@@ -1740,6 +1759,9 @@
         <v>18</v>
       </c>
       <c r="E62" t="s">
+        <v>18</v>
+      </c>
+      <c r="F62" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>

<commit_message>
NewFeature: - New: Add Lipid Master table generator in settings BugFix: - Fixed: TG Master table generation w/o O-/P- FA Improvements: - Improved: UI updates
</commit_message>
<xml_diff>
--- a/ConfigurationFiles/01-FA_Whitelist_TG-DG.xlsx
+++ b/ConfigurationFiles/01-FA_Whitelist_TG-DG.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{77F7DEFB-9296-4977-8EFA-7E678A4DE469}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20160" windowHeight="8475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20160" windowHeight="8475"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="69">
   <si>
     <t>FattyAcid</t>
   </si>
@@ -232,7 +231,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -543,11 +542,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B58" sqref="B57:B58"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="K50" sqref="K50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1691,9 +1690,6 @@
       <c r="E57" t="s">
         <v>18</v>
       </c>
-      <c r="F57" t="s">
-        <v>18</v>
-      </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
@@ -1705,9 +1701,6 @@
       <c r="E58" t="s">
         <v>18</v>
       </c>
-      <c r="F58" t="s">
-        <v>18</v>
-      </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
@@ -1719,9 +1712,6 @@
       <c r="E59" t="s">
         <v>18</v>
       </c>
-      <c r="F59" t="s">
-        <v>18</v>
-      </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
@@ -1733,9 +1723,6 @@
       <c r="E60" t="s">
         <v>18</v>
       </c>
-      <c r="F60" t="s">
-        <v>18</v>
-      </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
@@ -1747,9 +1734,6 @@
       <c r="E61" t="s">
         <v>18</v>
       </c>
-      <c r="F61" t="s">
-        <v>18</v>
-      </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
@@ -1759,9 +1743,6 @@
         <v>18</v>
       </c>
       <c r="E62" t="s">
-        <v>18</v>
-      </c>
-      <c r="F62" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Improvements: - Improved: UI elements rearranged for better user experience Changes: - Renamed: reorder of default config files to match UI changes
</commit_message>
<xml_diff>
--- a/ConfigurationFiles/01-FA_Whitelist_TG-DG.xlsx
+++ b/ConfigurationFiles/01-FA_Whitelist_TG-DG.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{23482CFD-157D-417E-843C-C50E488C9BF9}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20160" windowHeight="8475"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20160" windowHeight="8475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="69">
   <si>
     <t>FattyAcid</t>
   </si>
@@ -231,7 +232,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -542,11 +543,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="K50" sqref="K50"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="F56" sqref="F56:F62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1690,6 +1691,9 @@
       <c r="E57" t="s">
         <v>18</v>
       </c>
+      <c r="F57" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
@@ -1701,6 +1705,9 @@
       <c r="E58" t="s">
         <v>18</v>
       </c>
+      <c r="F58" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
@@ -1712,6 +1719,9 @@
       <c r="E59" t="s">
         <v>18</v>
       </c>
+      <c r="F59" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
@@ -1723,6 +1733,9 @@
       <c r="E60" t="s">
         <v>18</v>
       </c>
+      <c r="F60" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
@@ -1734,6 +1747,9 @@
       <c r="E61" t="s">
         <v>18</v>
       </c>
+      <c r="F61" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
@@ -1743,6 +1759,9 @@
         <v>18</v>
       </c>
       <c r="E62" t="s">
+        <v>18</v>
+      </c>
+      <c r="F62" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>